<commit_message>
finally found one of the bugs, w was being corrected for violations in excess of +/- pi, which should only be performed on angles, not angular rates. fixing this made it much closer to stable, but something is still wrong.
</commit_message>
<xml_diff>
--- a/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCm0.xlsx
+++ b/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCm0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\Crash-Sat\Crash-Sat\Aero design\Flight sim\hover stage sim - RK4 method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EAC3F2-A1F6-49FB-81C8-2B2A8988CCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773AB2DF-74F6-4E68-8EAE-CB090B193CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="2508" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="624" yWindow="2160" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:H14"/>
+      <selection sqref="A1:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -361,366 +361,366 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H13">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="B14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
very close to stable. problem seems to occur when theta loops around 180 degrees for some reason
</commit_message>
<xml_diff>
--- a/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCm0.xlsx
+++ b/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCm0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\Crash-Sat\Crash-Sat\Aero design\Flight sim\hover stage sim - RK4 method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773AB2DF-74F6-4E68-8EAE-CB090B193CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33F24F4-F19A-4A5B-A266-DFC9EEEE3103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="624" yWindow="2160" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,371 +356,372 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H1">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H9">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H10">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H11">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H12">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H13">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="D14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="E14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="G14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
       <c r="H14">
-        <v>0.5</v>
+        <v>3.048E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>